<commit_message>
commit the final code
</commit_message>
<xml_diff>
--- a/Resources/FeatureInput.xlsx
+++ b/Resources/FeatureInput.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Scenario</t>
   </si>
@@ -562,7 +562,7 @@
         <v>24</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>